<commit_message>
Uploaded more surfaces images.
</commit_message>
<xml_diff>
--- a/iSurfer/Galleries/Fuentes.xlsx
+++ b/iSurfer/Galleries/Fuentes.xlsx
@@ -78,9 +78,6 @@
     <t>interseccion</t>
   </si>
   <si>
-    <t>pera</t>
-  </si>
-  <si>
     <t>Advanced</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Vis a vis</t>
   </si>
   <si>
-    <t>Spitz</t>
-  </si>
-  <si>
     <t>Calypso</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>Nepali</t>
   </si>
   <si>
-    <t>Schneeflocke</t>
-  </si>
-  <si>
     <t>Expert</t>
   </si>
   <si>
@@ -160,6 +151,15 @@
   </si>
   <si>
     <t>Harlekin</t>
+  </si>
+  <si>
+    <t>Dromedar</t>
+  </si>
+  <si>
+    <t>Zeppelin</t>
+  </si>
+  <si>
+    <t>Pacman</t>
   </si>
 </sst>
 </file>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -740,7 +740,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3"/>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -765,7 +765,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -824,7 +824,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -833,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -842,7 +842,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -851,7 +851,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -860,7 +860,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -869,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -887,7 +887,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -896,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F20" s="3"/>
     </row>
@@ -905,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -914,7 +914,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -923,7 +923,7 @@
         <v>7</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -932,7 +932,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -941,7 +941,7 @@
         <v>8</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -950,7 +950,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -959,7 +959,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -968,7 +968,7 @@
         <v>5</v>
       </c>
       <c r="E24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -977,7 +977,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1027,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -1041,12 +1041,12 @@
         <v>2</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F30" s="3"/>
     </row>
@@ -1055,12 +1055,12 @@
         <v>3</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F31" s="3"/>
     </row>
@@ -1069,12 +1069,12 @@
         <v>4</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F32" s="3"/>
     </row>
@@ -1083,12 +1083,12 @@
         <v>5</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F33" s="3"/>
     </row>

</xml_diff>